<commit_message>
Adding real ball caster
</commit_message>
<xml_diff>
--- a/2014/ldd/BaseModel1/BaseModel1.xlsx
+++ b/2014/ldd/BaseModel1/BaseModel1.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Brick</t>
   </si>
@@ -47,6 +47,12 @@
     <t>26 - Black</t>
   </si>
   <si>
+    <t>STEEL BALL</t>
+  </si>
+  <si>
+    <t>21 - Bright Red</t>
+  </si>
+  <si>
     <t>6024581</t>
   </si>
   <si>
@@ -89,12 +95,6 @@
     <t>24 - Bright Yellow</t>
   </si>
   <si>
-    <t>4211375</t>
-  </si>
-  <si>
-    <t>BALL W. CROSS AXLE</t>
-  </si>
-  <si>
     <t>4121715</t>
   </si>
   <si>
@@ -114,12 +114,6 @@
   </si>
   <si>
     <t>23 - Bright Blue</t>
-  </si>
-  <si>
-    <t>4107083</t>
-  </si>
-  <si>
-    <t>CROSS AXLE, EXTENSION M/3 RIBS</t>
   </si>
   <si>
     <t>4211805</t>
@@ -265,7 +259,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="6024581 Screenshot" descr="6024581"/>
+        <xdr:cNvPr id="4" name=" Screenshot" descr=""/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -309,7 +303,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="6057952 Screenshot" descr="6057952"/>
+        <xdr:cNvPr id="5" name="6024581 Screenshot" descr="6024581"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -353,7 +347,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="6009996 Screenshot" descr="6009996"/>
+        <xdr:cNvPr id="6" name="6057952 Screenshot" descr="6057952"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -397,7 +391,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="4522934 Screenshot" descr="4522934"/>
+        <xdr:cNvPr id="7" name="6009996 Screenshot" descr="6009996"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -441,7 +435,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="4239601 Screenshot" descr="4239601"/>
+        <xdr:cNvPr id="8" name="4522934 Screenshot" descr="4522934"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -485,7 +479,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="4211375 Screenshot" descr="4211375"/>
+        <xdr:cNvPr id="9" name="4239601 Screenshot" descr="4239601"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -661,7 +655,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="4107083 Screenshot" descr="4107083"/>
+        <xdr:cNvPr id="13" name="4211805 Screenshot" descr="4211805"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -705,7 +699,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="4211805 Screenshot" descr="4211805"/>
+        <xdr:cNvPr id="14" name="4225033 Screenshot" descr="4225033"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -749,7 +743,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="4225033 Screenshot" descr="4225033"/>
+        <xdr:cNvPr id="15" name="4610380 Screenshot" descr="4610380"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -793,7 +787,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="4610380 Screenshot" descr="4610380"/>
+        <xdr:cNvPr id="16" name="4539880 Screenshot" descr="4539880"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -837,7 +831,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="4539880 Screenshot" descr="4539880"/>
+        <xdr:cNvPr id="17" name="4540797 Screenshot" descr="4540797"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -857,50 +851,6 @@
       <xdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="3448050" y="13611225"/>
-          <a:ext cx="813600" cy="813600"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>812800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="4540797 Screenshot" descr="4540797"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image17">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3448050" y="14449425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -915,7 +865,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -982,17 +932,14 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="66" customHeight="1">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>99948</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4">
-        <v>11145</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1000,16 +947,16 @@
     </row>
     <row r="5" spans="1:6" ht="66" customHeight="1">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5">
+        <v>11145</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5">
-        <v>95658</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1017,36 +964,36 @@
     </row>
     <row r="6" spans="1:6" ht="66" customHeight="1">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6">
+        <v>95658</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
-        <v>95646</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="66" customHeight="1">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7">
+        <v>95646</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
-        <v>41239</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
       <c r="F7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="66" customHeight="1">
@@ -1057,10 +1004,10 @@
         <v>24</v>
       </c>
       <c r="D8">
-        <v>32123</v>
+        <v>41239</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1068,19 +1015,19 @@
     </row>
     <row r="9" spans="1:6" ht="66" customHeight="1">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9">
+        <v>32123</v>
+      </c>
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="D9">
-        <v>2736</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
       <c r="F9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="66" customHeight="1">
@@ -1131,7 +1078,7 @@
         <v>34</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="66" customHeight="1">
@@ -1142,10 +1089,10 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <v>6538</v>
+        <v>44294</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1159,13 +1106,13 @@
         <v>38</v>
       </c>
       <c r="D14">
-        <v>44294</v>
+        <v>48989</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="66" customHeight="1">
@@ -1176,30 +1123,30 @@
         <v>40</v>
       </c>
       <c r="D15">
-        <v>48989</v>
+        <v>92911</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="66" customHeight="1">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>92911</v>
+        <v>64179</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="66" customHeight="1">
@@ -1210,38 +1157,21 @@
         <v>45</v>
       </c>
       <c r="D17">
-        <v>64179</v>
+        <v>64178</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="66" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18">
-        <v>64178</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
       <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19">
-        <f>SUM(F2:F18)</f>
+        <f>SUM(F2:F17)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>